<commit_message>
Concept identifier -> notation
</commit_message>
<xml_diff>
--- a/templates/VocExcel-template-060.xlsx
+++ b/templates/VocExcel-template-060.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/rdflib/VocExcel/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEABBBCA-8E3F-A24A-A7D4-5A1B67CBC9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92B5302-8C73-C943-B8FB-BCC29AB41DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>Version:</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>The Concept Scheme sheet stores basic metadata for the vocabulary as a whole. Each element has notes for its use on the Concept Scheme sheet itself.</t>
-  </si>
-  <si>
-    <t>SKOS Mapping properties, i.e. how Concepts listed in the Concepts sheet relate to Concepts in other vocabularies.</t>
   </si>
   <si>
     <t>Cross-cutting collections of Concepts. These allow you to group Concepts in ways differently to the main ConceptScheme that you create them in.</t>
@@ -706,19 +703,10 @@
     <t>A statement about the origin of this vocabulary</t>
   </si>
   <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>Identifier Type</t>
-  </si>
-  <si>
     <t>A textual ID for this Concept</t>
   </si>
   <si>
     <t>Must be present in Sheet Concepts &gt; Column A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If an Identifier is given, define the type </t>
   </si>
   <si>
     <t>IRI for this vocabulary. See the Documentation Sheet's IRI section</t>
@@ -775,6 +763,34 @@
   </si>
   <si>
     <t>0.6.0</t>
+  </si>
+  <si>
+    <t>Notation</t>
+  </si>
+  <si>
+    <t>Notation Type</t>
+  </si>
+  <si>
+    <t>GEO</t>
+  </si>
+  <si>
+    <t>http://example.com/dummy-id-regime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.org/au-research/vocabulary/anzsrc-for/2008/0403 </t>
+  </si>
+  <si>
+    <t>If a Notation is given, define the type by providing an IRI that identifies the ID management regime</t>
+  </si>
+  <si>
+    <t>SKOS Mapping properties, i.e. how Concepts listed in the Concepts sheet relate to Concepts in other vocabularies.
+If you want to supply multiple values for a concept, such as multiple Related Match IRIs or multiple Notations, just add in two rows with the same Concept IRI and distinct values in the appropriate field.</t>
+  </si>
+  <si>
+    <t>geol</t>
+  </si>
+  <si>
+    <t>http://example.com/another-dummy-id-regime</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1160,6 +1176,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1181,17 +1209,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1439,238 +1458,238 @@
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.15"/>
     <row r="3" spans="1:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
     </row>
     <row r="4" spans="1:10" ht="38" x14ac:dyDescent="0.15">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
+      <c r="E4" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
     </row>
     <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
     </row>
     <row r="6" spans="1:10" ht="38" x14ac:dyDescent="0.15">
-      <c r="A6" s="59"/>
-      <c r="B6" s="60" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+    </row>
+    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.15">
+      <c r="A7" s="52"/>
+      <c r="B7" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+    </row>
+    <row r="8" spans="1:10" ht="38" x14ac:dyDescent="0.15">
+      <c r="A8" s="52"/>
+      <c r="B8" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.15">
+      <c r="A9" s="52"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+    </row>
+    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.15">
+      <c r="A10" s="52"/>
+      <c r="B10" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-    </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.15">
-      <c r="A7" s="59"/>
-      <c r="B7" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-    </row>
-    <row r="8" spans="1:10" ht="38" x14ac:dyDescent="0.15">
-      <c r="A8" s="59"/>
-      <c r="B8" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A9" s="59"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-    </row>
-    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.15">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.15">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+    </row>
+    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="52"/>
+      <c r="B12" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-    </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-    </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60" t="s">
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+    </row>
+    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.15">
+      <c r="A13" s="52"/>
+      <c r="B13" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-    </row>
-    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.15">
-      <c r="A13" s="59"/>
-      <c r="B13" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A14" s="59"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
     </row>
     <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
     </row>
     <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A16" s="59"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A17" s="59"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
     </row>
     <row r="18" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A18" s="59"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
     </row>
     <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="59"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
     </row>
     <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.15"/>
     <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.15"/>
@@ -2653,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E056D66-684B-EA44-9D39-98A26FD38952}">
   <dimension ref="A2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.15"/>
@@ -2672,47 +2691,47 @@
     </row>
     <row r="3" spans="1:3" ht="209" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="364" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="211" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="97" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="B7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="8"/>
     </row>
@@ -2734,7 +2753,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -2742,12 +2761,12 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="114" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -2760,7 +2779,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3"/>
     </row>
@@ -2770,10 +2789,10 @@
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -2806,25 +2825,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.15">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" s="46" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -2833,7 +2852,7 @@
       </c>
       <c r="B3" s="47"/>
       <c r="C3" s="44" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>27</v>
@@ -2857,7 +2876,7 @@
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>3</v>
@@ -2929,7 +2948,7 @@
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="44" t="s">
         <v>3</v>
@@ -5924,7 +5943,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.15"/>
@@ -5941,20 +5960,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.15">
       <c r="A2" s="42" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" s="42" t="s">
         <v>17</v>
@@ -5966,84 +5985,84 @@
         <v>19</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="43" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H2" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="C3" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="32" t="s">
+      <c r="G3" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="H3" s="32" t="s">
         <v>82</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="133" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="C4" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>70</v>
-      </c>
       <c r="E4" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="95" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>72</v>
-      </c>
       <c r="C5" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="76" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6065,11 +6084,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6077,51 +6096,51 @@
     <col min="1" max="1" width="33.5" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="25.1640625" style="19" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="19" customWidth="1"/>
     <col min="9" max="16384" width="12.5" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
     </row>
     <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="37" t="s">
-        <v>52</v>
-      </c>
       <c r="E2" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="37" t="s">
+    </row>
+    <row r="3" spans="1:27" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
         <v>98</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="35" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
-        <v>101</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -6129,10 +6148,10 @@
       <c r="E3" s="39"/>
       <c r="F3" s="39"/>
       <c r="G3" s="38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
@@ -6154,7 +6173,23 @@
       <c r="Z3" s="34"/>
       <c r="AA3" s="34"/>
     </row>
-    <row r="4" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>120</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -6175,11 +6210,30 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
     </row>
+    <row r="5" spans="1:27" ht="38" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="63" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{4FF6A4FF-528E-9942-9893-F27DAA2099BC}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{F0D0EE91-714A-3F4E-A186-3B8BE81D2EA0}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{09E6D447-8752-0E4E-97D3-CD14C873DDA9}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{ED9F9511-2579-A64A-81E3-D849D16BA929}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{2DB04D9F-13CA-5044-B200-ED9575186A93}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6206,17 +6260,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>17</v>
@@ -6225,7 +6279,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>20</v>
@@ -6236,25 +6290,25 @@
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
       <c r="D3" s="51" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="D4" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7631,7 +7685,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -7644,11 +7698,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="A1" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="29" t="s">
@@ -7658,7 +7712,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="24"/>
     </row>
@@ -7667,30 +7721,30 @@
         <v>25</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>90</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="C5" s="24" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>94</v>
       </c>
       <c r="D5" s="24"/>
     </row>

</xml_diff>